<commit_message>
fix a bug of Annotation Class URI :annotation -> :Annotation
</commit_message>
<xml_diff>
--- a/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
+++ b/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SURFACEPRO4-NOR\data\metadb\OME\xml2RDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F8B274-02AE-4700-B8FF-F19701512708}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B5DC07-44EC-4FAD-BFE7-EC6E8A1F03ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34500" windowHeight="5025" xr2:uid="{C6590354-B643-425C-8354-6D133489F49F}"/>
   </bookViews>
@@ -1811,9 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E08185-2587-4456-8CBB-2A2DBF78CD1C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1857,7 +1855,7 @@
         <v>140</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
fix some errors and supports the ome_unit ontology
</commit_message>
<xml_diff>
--- a/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
+++ b/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SURFACEPRO4-NOR\data\metadb\OME\xml2RDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\metadb\OME\xml2RDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B5DC07-44EC-4FAD-BFE7-EC6E8A1F03ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFB3E39-D198-4875-8846-CBC08F98CAD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34500" windowHeight="5025" xr2:uid="{C6590354-B643-425C-8354-6D133489F49F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34500" windowHeight="5028" xr2:uid="{C6590354-B643-425C-8354-6D133489F49F}"/>
   </bookViews>
   <sheets>
     <sheet name="@prefix" sheetId="8" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="Binary_Data" sheetId="13" r:id="rId6"/>
     <sheet name="Structured_Annotations" sheetId="21" r:id="rId7"/>
     <sheet name="Comment_Annotation" sheetId="15" r:id="rId8"/>
-    <sheet name="Unit" sheetId="19" r:id="rId9"/>
-    <sheet name="size" sheetId="20" r:id="rId10"/>
+    <sheet name="size" sheetId="20" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="132">
   <si>
     <t/>
   </si>
@@ -370,10 +369,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>xsd:string</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>pixelType</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -389,9 +384,6 @@
     <t>Annotation:1</t>
   </si>
   <si>
-    <t>Fred</t>
-  </si>
-  <si>
     <t>Channel:0</t>
   </si>
   <si>
@@ -399,18 +391,6 @@
   </si>
   <si>
     <t>Image:0</t>
-  </si>
-  <si>
-    <t>Unit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>prefix</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>base unit</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>単位</t>
@@ -420,63 +400,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>名称</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>接頭辞</t>
-    <rPh sb="0" eb="3">
-      <t>セットウジ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>基本単位</t>
-    <rPh sb="0" eb="2">
-      <t>キホン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>タンイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:prefix</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:baseUnit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:Unit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>UO:0000046</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>UO:0000000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>unit:nm</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>"nano-meter"@en</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>UO:0000300</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>UO:0000008</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Size</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -511,14 +434,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>unit:um</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/unit/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>PATO</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -567,6 +482,25 @@
   </si>
   <si>
     <t>:Annotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xsd:langString</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>"Fred"@en</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>unitLength:nm</t>
+  </si>
+  <si>
+    <t>unitLength</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/Unit/UnitLength#</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -574,7 +508,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,13 +549,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -684,11 +611,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,14 +939,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1043,7 +970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1075,39 +1002,39 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+        <v>116</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1115,7 +1042,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1123,100 +1050,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D5DD21-DCFD-4C99-9450-C1B8BA0B1274}">
-  <sheetPr>
-    <tabColor theme="4" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5">
-        <v>100000</v>
-      </c>
-      <c r="D5" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1233,19 +1071,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1265,10 +1103,10 @@
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1281,7 +1119,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1299,10 +1137,10 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1322,15 +1160,15 @@
         <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>58</v>
@@ -1358,21 +1196,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="17.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.69921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1221,7 @@
         <v>50</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>35</v>
@@ -1416,7 +1254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1272,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
@@ -1443,7 +1281,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>67</v>
@@ -1476,7 +1314,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1493,10 +1331,10 @@
         <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>41</v>
@@ -1520,12 +1358,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>64</v>
@@ -1534,10 +1372,10 @@
         <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1574,16 +1412,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1597,7 +1435,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1605,7 +1443,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1617,7 +1455,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1631,12 +1469,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>90</v>
@@ -1654,15 +1492,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1673,14 +1511,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1689,7 +1527,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1700,7 +1538,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>90</v>
       </c>
@@ -1720,16 +1558,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1746,7 +1584,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1755,7 +1593,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1770,7 +1608,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1784,10 +1622,10 @@
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>79</v>
       </c>
@@ -1813,54 +1651,54 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>81</v>
@@ -1879,16 +1717,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.75" style="1"/>
+    <col min="4" max="4" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1902,7 +1740,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1910,7 +1748,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1922,7 +1760,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1933,18 +1771,18 @@
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1954,104 +1792,90 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EBD5A9-A917-4160-97D9-377E7FDDD01B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D5DD21-DCFD-4C99-9450-C1B8BA0B1274}">
   <sheetPr>
-    <tabColor theme="4" tint="0.39997558519241921"/>
+    <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>122</v>
+        <v>60</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5">
+        <v>100000</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed some errors on Medium and NamingConvention
</commit_message>
<xml_diff>
--- a/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
+++ b/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\metadb\OME\xml2RDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFB3E39-D198-4875-8846-CBC08F98CAD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F4E355-4E51-4880-9E68-82480459C169}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34500" windowHeight="5028" xr2:uid="{C6590354-B643-425C-8354-6D133489F49F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="140">
   <si>
     <t/>
   </si>
@@ -203,10 +203,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>[pixels:0:0]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>dimensionOrder</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -300,18 +296,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>[bindata:0]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/image/</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>[commentAnnoation:1]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>channel</t>
   </si>
   <si>
@@ -339,10 +327,6 @@
   </si>
   <si>
     <t>[color:-2147483648]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[channel:0]</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -493,14 +477,63 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>unitLength:nm</t>
-  </si>
-  <si>
     <t>unitLength</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/Unit/UnitLength#</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>pixels</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/pixels/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>channel</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/channel/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bindata</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/bindata/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>commentAnnotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/samples/commentannotation/commentAnnoation/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>channel:channel0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bindata:bindata0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>pixels:pixels0.0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>commentAnnotation:commentAnnotation1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>unitLength:um</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -935,14 +968,14 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1004,58 +1037,90 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>131</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1079,7 +1144,7 @@
     <col min="4" max="4" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1103,7 +1168,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1137,7 +1202,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -1160,7 +1225,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -1168,19 +1233,19 @@
         <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1199,14 +1264,14 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="17.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.69921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1221,7 +1286,7 @@
         <v>50</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>35</v>
@@ -1248,7 +1313,7 @@
         <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>34</v>
@@ -1281,37 +1346,37 @@
         <v>51</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -1319,22 +1384,22 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>41</v>
@@ -1352,30 +1417,30 @@
         <v>41</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N4" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="B5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1393,10 +1458,10 @@
         <v>1</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +1480,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
@@ -1426,13 +1491,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1452,7 +1517,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1460,24 +1525,24 @@
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="1" t="s">
-        <v>91</v>
+      <c r="B5" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1505,10 +1570,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1524,7 +1589,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1532,7 +1597,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>52</v>
@@ -1540,7 +1605,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1">
         <v>-2147483648</v>
@@ -1561,7 +1626,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
@@ -1581,7 +1647,7 @@
         <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1605,7 +1671,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1622,18 +1688,18 @@
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1">
         <v>32</v>
@@ -1655,7 +1721,7 @@
   <cols>
     <col min="1" max="1" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -1663,10 +1729,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1682,7 +1748,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1690,18 +1756,18 @@
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1786,7 @@
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.69921875" style="1"/>
@@ -1731,13 +1797,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1757,7 +1823,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1765,24 +1831,24 @@
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1813,13 +1879,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1827,13 +1893,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1842,10 +1908,10 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1853,24 +1919,24 @@
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5">
         <v>100000</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redefined prefix "ome" instead of ":" (base prefix name).
</commit_message>
<xml_diff>
--- a/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
+++ b/ontology/RIKEN_MetaDatabase_Exccel/2016-06/sample/commentannotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\metadb\OME\xml2RDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F4E355-4E51-4880-9E68-82480459C169}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03B0732-E7A2-4D6B-AC78-6EE1654F2348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34500" windowHeight="5028" xr2:uid="{C6590354-B643-425C-8354-6D133489F49F}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="140">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="138">
   <si>
     <t>http://www.openmicroscopy.org/rdf/2016-06/ome_core/</t>
   </si>
@@ -98,24 +95,12 @@
     <t>rdfs:label</t>
   </si>
   <si>
-    <t>:pixels</t>
-  </si>
-  <si>
-    <t>:acquisitionDate</t>
-  </si>
-  <si>
     <t>datatype</t>
   </si>
   <si>
-    <t>:Image</t>
-  </si>
-  <si>
     <t>rdf:langString</t>
   </si>
   <si>
-    <t>:Pixels</t>
-  </si>
-  <si>
     <t>xsd:dateTime</t>
   </si>
   <si>
@@ -152,27 +137,18 @@
     <t>size y</t>
   </si>
   <si>
-    <t>:bigEndian</t>
-  </si>
-  <si>
     <t>xsd:boolean</t>
   </si>
   <si>
     <t>xsd:positiveInteger</t>
   </si>
   <si>
-    <t>:BinData</t>
-  </si>
-  <si>
     <t>Binary Data</t>
   </si>
   <si>
     <t>data</t>
   </si>
   <si>
-    <t>:data</t>
-  </si>
-  <si>
     <t>xsd:base64Binary</t>
   </si>
   <si>
@@ -211,10 +187,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:length</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>"6x6x1x8-swatch.tif"@en</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -240,58 +212,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:Pixels</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:PixelType</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:dimensionOrder</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:DimensionOrder</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:physicalSizeX</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:physicalSizeY</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:sizeC</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:sizeT</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:sizeX</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:sizeY</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:sizeZ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:binData</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:BinData</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>dimensionOrder:xyczt</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -303,29 +223,12 @@
     <t>channel</t>
   </si>
   <si>
-    <t>channel</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Channel</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Channel</t>
   </si>
   <si>
     <t>color</t>
   </si>
   <si>
-    <t>:color</t>
-  </si>
-  <si>
-    <t>:Channel</t>
-  </si>
-  <si>
-    <t>:Color</t>
-  </si>
-  <si>
     <t>[color:-2147483648]</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -345,10 +248,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:CommentAnnotation</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>comment annotation value</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -358,10 +257,6 @@
   </si>
   <si>
     <t>pixel type</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>:pixelType</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -445,18 +340,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:StructuredAnnotations</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>annotation</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:annotation</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>[structuredAnnotation:0]</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -465,10 +352,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>:Annotation</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>xsd:langString</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -534,6 +417,126 @@
   </si>
   <si>
     <t>unitLength:um</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Image</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:pixels</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:acquisitionDate</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:annotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Annotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Pixels</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:pixelType</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:dimensionOrder</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:DimensionOrder</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:physicalSizeX</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:sizeC</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:sizeT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:sizeX</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:sizeY</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:sizeZ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:channel</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Channel</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:binData</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:BinData</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Channel</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:color</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:Color</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:BinData</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:bigEndian</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:data</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:length</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:StructuredAnnotations</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:CommentAnnotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ome:physicalSizeY</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -981,146 +984,146 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1142,43 +1145,43 @@
     <col min="2" max="2" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1186,66 +1189,66 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1264,11 +1267,12 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.8984375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="17.5" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" style="6" bestFit="1" customWidth="1"/>
@@ -1277,51 +1281,51 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1339,108 +1343,108 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1458,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1481,28 +1485,28 @@
   <cols>
     <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1510,39 +1514,39 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1567,45 +1571,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1">
         <v>-2147483648</v>
@@ -1627,32 +1631,32 @@
   <cols>
     <col min="1" max="1" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1661,45 +1665,45 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1">
         <v>32</v>
@@ -1719,55 +1723,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1794,21 +1798,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1816,39 +1820,39 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1876,67 +1880,67 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>100000</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>